<commit_message>
เพิ่ม Automate Test ของ Admin
</commit_message>
<xml_diff>
--- a/Admin/test_login/test_data.xlsx
+++ b/Admin/test_login/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automate Test\Test_PMS\automateTestTeam0\Admin\test_login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30962FBF-3CA4-4A79-AC2D-F478A385F64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A283868-4F9C-4A84-8C66-6665AF5A9242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>'</t>
+  </si>
+  <si>
+    <t>kajorn</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>ฟ่นพื</t>
+  </si>
+  <si>
+    <t>testadmin@gmail.com</t>
+  </si>
+  <si>
+    <t>kjorn</t>
   </si>
 </sst>
 </file>
@@ -417,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +541,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,24 +564,45 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -577,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4469ECF-F093-4766-862D-03DA52484F9E}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,27 +636,82 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{136BEE20-0563-415B-AD06-2F61B3AF84F1}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{61D00682-520E-4D75-BF8F-CE1113FCD9F4}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{8114A590-DB4A-4C29-A302-C4B9CF9CD70F}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{6C02EAA8-F329-4333-9639-B3E7AFC1ED48}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{DE2D0092-CF19-4134-B8B8-A47FC6E6377C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>